<commit_message>
implement the two experiment with linear cost for line selection and quadratic cost
</commit_message>
<xml_diff>
--- a/InteropTest/InteropTest.xlsx
+++ b/InteropTest/InteropTest.xlsx
@@ -17,13 +17,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -421,7 +427,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,7 +442,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="1025" r:id="rId4" name="Button 1">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.SelectEvenLines">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="_xll.SelectLines">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>7</xdr:col>

</xml_diff>